<commit_message>
Fix minor bugs and add new layout sizes
</commit_message>
<xml_diff>
--- a/tom/Valid_Designs.xlsx
+++ b/tom/Valid_Designs.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomka\Desktop\Winter Quarter 2019\MAE 154A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Desktop\MAE154A_UAVDesign-master\tom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0B3CCE1-28D0-49A4-9AF5-13FAD997B7BB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="230" windowWidth="12110" windowHeight="9970" xr2:uid="{913198AA-A050-429B-B483-58705045676F}"/>
+    <workbookView xWindow="6225" yWindow="225" windowWidth="12105" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -108,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,38 +452,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D9ECC7-9C5D-47DF-A6F7-FD6D1174EAE8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -558,18 +556,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>14.297308003521049</v>
+        <v>13.668482276188673</v>
       </c>
       <c r="B2">
-        <v>0.98763254297768388</v>
+        <v>0.94576720880508192</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>9.1127009371980154</v>
+        <v>4.2293705710665854</v>
       </c>
       <c r="E2">
         <v>0.7</v>
@@ -587,7 +585,7 @@
         <v>4</v>
       </c>
       <c r="J2">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="K2">
         <v>0.5</v>
@@ -596,19 +594,19 @@
         <v>0.5</v>
       </c>
       <c r="M2">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="N2">
         <v>1.5</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P2">
         <v>1.5</v>
       </c>
       <c r="Q2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R2">
         <v>0.5</v>
@@ -623,13 +621,13 @@
         <v>2</v>
       </c>
       <c r="V2">
-        <v>14.476343560343885</v>
+        <v>14.452269172514399</v>
       </c>
       <c r="W2">
-        <v>0.12407045648527366</v>
+        <v>0.13367625320445395</v>
       </c>
       <c r="X2">
-        <v>1.7738735305074131</v>
+        <v>1.8271514976723882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>